<commit_message>
adding space, bos, and eos in atb3
</commit_message>
<xml_diff>
--- a/ExcelDocuments/arabic_diacritics.xlsx
+++ b/ExcelDocuments/arabic_diacritics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Magdy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\MST\MST\ExcelDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>ْ</t>
-  </si>
-  <si>
-    <t>ّ</t>
   </si>
   <si>
     <t>َّ</t>
@@ -426,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +499,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -510,7 +507,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -549,14 +546,6 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "adding space, bos, and eos in atb3"
This reverts commit 967236d0bf38b6b3ebbe93eeeb712fc3c07fe9a7.
</commit_message>
<xml_diff>
--- a/ExcelDocuments/arabic_diacritics.xlsx
+++ b/ExcelDocuments/arabic_diacritics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\MST\MST\ExcelDocuments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed Magdy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>ْ</t>
+  </si>
+  <si>
+    <t>ّ</t>
   </si>
   <si>
     <t>َّ</t>
@@ -423,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,7 +502,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -507,7 +510,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -546,6 +549,14 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>